<commit_message>
Phân quyền trên code backend + fix lỗi xuất pdf bị lỗi content not found
</commit_message>
<xml_diff>
--- a/static/web/excel/Data_Nhan_Vien.xlsx
+++ b/static/web/excel/Data_Nhan_Vien.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="133">
   <si>
     <t>TenNV</t>
   </si>
@@ -175,12 +175,15 @@
     <t>Chưa tốt nghiệp-Vật Lý</t>
   </si>
   <si>
+    <t>Làng sinh viên Hacinco - Nhân Chính - Thanh Xuân - Hà Nội</t>
+  </si>
+  <si>
+    <t>Hiệp Hòa - Bắc Giang</t>
+  </si>
+  <si>
     <t>Làng sinh viên Hacinco - Nhân Chính - Thanh Xuân - Hà Nội - Việt Nam</t>
   </si>
   <si>
-    <t>Hiệp Hòa - Bắc Giang</t>
-  </si>
-  <si>
     <t>Ha Noi</t>
   </si>
   <si>
@@ -271,7 +274,7 @@
     <t>0945875315</t>
   </si>
   <si>
-    <t>856865245</t>
+    <t>0856865245</t>
   </si>
   <si>
     <t>001205068139</t>
@@ -304,6 +307,9 @@
     <t>03-08-2020</t>
   </si>
   <si>
+    <t>12-12-2020</t>
+  </si>
+  <si>
     <t>03-05-2019</t>
   </si>
   <si>
@@ -317,6 +323,9 @@
   </si>
   <si>
     <t>Hiệp Hòa</t>
+  </si>
+  <si>
+    <t>Phú Thọ</t>
   </si>
   <si>
     <t>Bắc Giang</t>
@@ -846,37 +855,37 @@
         <v>53</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="P2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="Q2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="R2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -905,34 +914,34 @@
         <v>54</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N3" t="s">
         <v>54</v>
       </c>
       <c r="O3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="P3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="Q3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="R3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -955,40 +964,40 @@
         <v>1000000</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="P4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="Q4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="R4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1008,28 +1017,34 @@
         <v>50</v>
       </c>
       <c r="F5">
-        <v>0.25</v>
+        <v>1000000</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L5" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="M5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" t="s">
+        <v>103</v>
       </c>
       <c r="O5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="P5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1052,25 +1067,25 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="P6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1093,25 +1108,25 @@
         <v>0.3</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="P7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1134,25 +1149,25 @@
         <v>0.2</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="P8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1175,25 +1190,25 @@
         <v>0.15</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="P9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1216,31 +1231,31 @@
         <v>700000</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="N10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="O10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="P10" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1263,40 +1278,40 @@
         <v>20000000</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="P11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="Q11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1307,7 +1322,7 @@
         <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
@@ -1319,40 +1334,40 @@
         <v>1000000</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="N12" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="P12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="Q12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="R12" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1375,40 +1390,40 @@
         <v>950000</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M13" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="P13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="Q13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="R13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kiểm tra lại các template đã có và sửa một vài lỗi liên quan đến xuất file pdf
</commit_message>
<xml_diff>
--- a/static/web/excel/Data_Nhan_Vien.xlsx
+++ b/static/web/excel/Data_Nhan_Vien.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
   <si>
     <t>TenNV</t>
   </si>
@@ -115,10 +115,10 @@
     <t>Lã Đức Nam</t>
   </si>
   <si>
-    <t>Pham Hong Nghia</t>
-  </si>
-  <si>
-    <t>Pham Nhat Vuong</t>
+    <t>Phạm Hồng Nghĩa</t>
+  </si>
+  <si>
+    <t>Phạm Nhật Vượng</t>
   </si>
   <si>
     <t>Nguyen Khac Huy</t>
@@ -184,6 +184,12 @@
     <t>Làng sinh viên Hacinco - Nhân Chính - Thanh Xuân - Hà Nội - Việt Nam</t>
   </si>
   <si>
+    <t>36 Vũ Trọng Phụng, Thanh Xuân Trung, Thanh Xuân, Hà Nội</t>
+  </si>
+  <si>
+    <t>Phù Lưu, Lộc Hà, Hà Tĩnh</t>
+  </si>
+  <si>
     <t>Ha Noi</t>
   </si>
   <si>
@@ -196,6 +202,9 @@
     <t>Hà Tây</t>
   </si>
   <si>
+    <t>Phú Thọ</t>
+  </si>
+  <si>
     <t>Thôn Xuân Tân - Xuân Hưng - Thọ Xuân - Thanh Hoá  - Việt Nam</t>
   </si>
   <si>
@@ -217,24 +226,27 @@
     <t>04-04-2002</t>
   </si>
   <si>
+    <t>05-08-1968</t>
+  </si>
+  <si>
+    <t>01-10-2002</t>
+  </si>
+  <si>
+    <t>05-05-2002</t>
+  </si>
+  <si>
+    <t>05-08-2002</t>
+  </si>
+  <si>
+    <t>09-09-2002</t>
+  </si>
+  <si>
+    <t>14-02-2002</t>
+  </si>
+  <si>
     <t>07-07-2002</t>
   </si>
   <si>
-    <t>01-10-2002</t>
-  </si>
-  <si>
-    <t>05-05-2002</t>
-  </si>
-  <si>
-    <t>05-08-2002</t>
-  </si>
-  <si>
-    <t>09-09-2002</t>
-  </si>
-  <si>
-    <t>14-02-2002</t>
-  </si>
-  <si>
     <t>Nam</t>
   </si>
   <si>
@@ -289,6 +301,9 @@
     <t>123456789</t>
   </si>
   <si>
+    <t>000827826195</t>
+  </si>
+  <si>
     <t>001206064297</t>
   </si>
   <si>
@@ -310,6 +325,9 @@
     <t>12-12-2020</t>
   </si>
   <si>
+    <t>10-10-1986</t>
+  </si>
+  <si>
     <t>03-05-2019</t>
   </si>
   <si>
@@ -325,9 +343,6 @@
     <t>Hiệp Hòa</t>
   </si>
   <si>
-    <t>Phú Thọ</t>
-  </si>
-  <si>
     <t>Bắc Giang</t>
   </si>
   <si>
@@ -388,6 +403,9 @@
     <t>SV401985718</t>
   </si>
   <si>
+    <t>SV40101135729</t>
+  </si>
+  <si>
     <t>SV40101208765</t>
   </si>
   <si>
@@ -404,6 +422,9 @@
   </si>
   <si>
     <t>0118157171</t>
+  </si>
+  <si>
+    <t>0811002892</t>
   </si>
   <si>
     <t>0118000001</t>
@@ -855,37 +876,37 @@
         <v>53</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="M2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="N2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="O2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="Q2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="R2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -914,34 +935,34 @@
         <v>54</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="M3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="N3" t="s">
         <v>54</v>
       </c>
       <c r="O3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="P3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="Q3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="R3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -967,37 +988,37 @@
         <v>55</v>
       </c>
       <c r="H4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" t="s">
         <v>59</v>
       </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M4" t="s">
-        <v>96</v>
-      </c>
-      <c r="N4" t="s">
-        <v>57</v>
-      </c>
       <c r="O4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="P4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="Q4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="R4" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1022,29 +1043,38 @@
       <c r="G5" t="s">
         <v>56</v>
       </c>
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="M5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="N5" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="O5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P5" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>129</v>
+      </c>
+      <c r="R5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1064,28 +1094,37 @@
         <v>51</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>95</v>
+      </c>
+      <c r="M6" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" t="s">
+        <v>57</v>
       </c>
       <c r="O6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="P6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1108,25 +1147,25 @@
         <v>0.3</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P7" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1149,25 +1188,25 @@
         <v>0.2</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P8" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1190,25 +1229,25 @@
         <v>0.15</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="P9" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1231,31 +1270,31 @@
         <v>700000</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="M10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="N10" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="O10" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="P10" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1281,37 +1320,37 @@
         <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L11" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="M11" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="N11" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="O11" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="P11" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="Q11" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="R11" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1337,37 +1376,37 @@
         <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L12" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="M12" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="N12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="O12" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="P12" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="Q12" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="R12" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1390,40 +1429,40 @@
         <v>950000</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="L13" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="M13" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="N13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="O13" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="P13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="Q13" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="R13" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>